<commit_message>
Test Plan, Check List, Test Report
</commit_message>
<xml_diff>
--- a/week3/CheckList.xlsx
+++ b/week3/CheckList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -147,12 +147,15 @@
   <si>
     <t>Милота *_*</t>
   </si>
+  <si>
+    <t>Все проверки необходимо провести для каждого из браузеров, указанных в Тест-плане</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +168,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -191,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -201,6 +212,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -502,7 +514,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -516,104 +528,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>